<commit_message>
Added test that checks redirect to proper site in all subcategories
</commit_message>
<xml_diff>
--- a/src/test/resources/XKomData.xlsx
+++ b/src/test/resources/XKomData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
   <si>
     <t>menu_className</t>
   </si>
@@ -106,13 +106,214 @@
   </si>
   <si>
     <t>Kable i przejściówki</t>
+  </si>
+  <si>
+    <t>Laptopy 2 w 1</t>
+  </si>
+  <si>
+    <t>Tablety</t>
+  </si>
+  <si>
+    <t>Czytniki ebook</t>
+  </si>
+  <si>
+    <t>Torby i etui</t>
+  </si>
+  <si>
+    <t>Akcesoria do laptopów</t>
+  </si>
+  <si>
+    <t>Akcesoria do tabletów</t>
+  </si>
+  <si>
+    <t>Inteligentne zegarki</t>
+  </si>
+  <si>
+    <t>Nawigacje GPS</t>
+  </si>
+  <si>
+    <t>Wideorejestratory</t>
+  </si>
+  <si>
+    <t>Pamięci flash</t>
+  </si>
+  <si>
+    <t>Drony</t>
+  </si>
+  <si>
+    <t>Urządzenia multimedialne</t>
+  </si>
+  <si>
+    <t>Akcesoria GSM</t>
+  </si>
+  <si>
+    <t>Akcesoria GPS</t>
+  </si>
+  <si>
+    <t>Akcesoria do dronów</t>
+  </si>
+  <si>
+    <t>Akcesoria komputerowe</t>
+  </si>
+  <si>
+    <t>Akcesoria do monitorów</t>
+  </si>
+  <si>
+    <t>Karty graficzne</t>
+  </si>
+  <si>
+    <t>Procesory</t>
+  </si>
+  <si>
+    <t>Płyty główne</t>
+  </si>
+  <si>
+    <t>Pamięci RAM</t>
+  </si>
+  <si>
+    <t>Obudowy komputerowe</t>
+  </si>
+  <si>
+    <t>Zasilacze komputerowe</t>
+  </si>
+  <si>
+    <t>Chłodzenia komputerowe</t>
+  </si>
+  <si>
+    <t>Tuning PC</t>
+  </si>
+  <si>
+    <t>Karty dźwiękowe</t>
+  </si>
+  <si>
+    <t>Karty video</t>
+  </si>
+  <si>
+    <t>Pokaż wszystkie</t>
+  </si>
+  <si>
+    <t>Urządzenia wielofunkcyjne</t>
+  </si>
+  <si>
+    <t>Drukarki</t>
+  </si>
+  <si>
+    <t>Urządzenia sieciowe</t>
+  </si>
+  <si>
+    <t>Myszki</t>
+  </si>
+  <si>
+    <t>Klawiatury</t>
+  </si>
+  <si>
+    <t>Słuchawki i mikrofony</t>
+  </si>
+  <si>
+    <t>Głośniki</t>
+  </si>
+  <si>
+    <t>Projektory i ekrany</t>
+  </si>
+  <si>
+    <t>Skanery</t>
+  </si>
+  <si>
+    <t>Tablety graficzne</t>
+  </si>
+  <si>
+    <t>Komputery do gier</t>
+  </si>
+  <si>
+    <t>Podzespoły do gier</t>
+  </si>
+  <si>
+    <t>Myszki i klawiatury dla graczy</t>
+  </si>
+  <si>
+    <t>Monitory dla graczy</t>
+  </si>
+  <si>
+    <t>Audio dla graczy</t>
+  </si>
+  <si>
+    <t>Konsole</t>
+  </si>
+  <si>
+    <t>Akcesoria do konsol</t>
+  </si>
+  <si>
+    <t>Gry</t>
+  </si>
+  <si>
+    <t>Kontrolery do gier</t>
+  </si>
+  <si>
+    <t>Fotele dla graczy</t>
+  </si>
+  <si>
+    <t>Kino domowe</t>
+  </si>
+  <si>
+    <t>Hi-Fi audio</t>
+  </si>
+  <si>
+    <t>Kolumny głośnikowe</t>
+  </si>
+  <si>
+    <t>Przenośny sprzęt audio</t>
+  </si>
+  <si>
+    <t>Power Audio</t>
+  </si>
+  <si>
+    <t>Aparaty fotograficzne</t>
+  </si>
+  <si>
+    <t>Kamery</t>
+  </si>
+  <si>
+    <t>Programy biurowe</t>
+  </si>
+  <si>
+    <t>Programy antywirusowe</t>
+  </si>
+  <si>
+    <t>Programy graficzne i wideo</t>
+  </si>
+  <si>
+    <t>Programy użytkowe</t>
+  </si>
+  <si>
+    <t>Systemy sprzedaży</t>
+  </si>
+  <si>
+    <t>Kontrola rodzicielska</t>
+  </si>
+  <si>
+    <t>Zasilanie</t>
+  </si>
+  <si>
+    <t>Nośniki i akcesoria</t>
+  </si>
+  <si>
+    <t>Czytniki kart pamięci</t>
+  </si>
+  <si>
+    <t>Dyski zewnętrzne i przenośne</t>
+  </si>
+  <si>
+    <t>Pojazdy elektryczne</t>
+  </si>
+  <si>
+    <t>hidden_menu_subcategory_quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +333,13 @@
       <name val="Consolas"/>
       <family val="3"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,12 +362,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -461,126 +670,419 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
-    <col min="2" max="2" width="74.5703125" customWidth="1"/>
+    <col min="1" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="74.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="E6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="E7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>